<commit_message>
added features to backlog
</commit_message>
<xml_diff>
--- a/documentation/Feature brainstorm.xlsx
+++ b/documentation/Feature brainstorm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ALTUSER\Documents\Koodiprojektit\Kotkan meripaeivaet\kotkan-meripaevaet\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE0439D4-2492-4375-AF21-8466B1CB34A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D737FEE7-D2BE-4189-8F27-017EA0849BBC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="2565" windowWidth="21600" windowHeight="11385" xr2:uid="{2259D7AB-64B9-473A-AB4C-7A1A3C4987B4}"/>
+    <workbookView xWindow="3810" yWindow="1695" windowWidth="21600" windowHeight="12885" xr2:uid="{2259D7AB-64B9-473A-AB4C-7A1A3C4987B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>Feature Brainstorm</t>
   </si>
@@ -76,6 +76,24 @@
   </si>
   <si>
     <t>Pystyy tekemään kiireluonteisen ilmoituksen tapaturman tai muun odottamattoman seikan johdosta. Sovellus pyrkii herjaamaan käyttäjiä, kunnes he ilmoittavat nähneensä panic ilmoituksen</t>
+  </si>
+  <si>
+    <t>Ihmisten ryhmittyminen kartalla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jos yhdellä alueella on paljon käyttäjiä, käyttäjien kuvakkeet sulautuvat palloon, josta käy ilmi pienellä alueella olevien käyttäjien määrä. </t>
+  </si>
+  <si>
+    <t>Ryhmään liittyminen ilman käyttäjää</t>
+  </si>
+  <si>
+    <t>Jos käyttäjä unohtaa kirjautumistietonsa, hän voi liittyä vieraskäyttäjänä ryhmään ryhmän nimen ja salasanan avulla.</t>
+  </si>
+  <si>
+    <t>Layers-valikosta voi piilottaa/näyttää kartan ikonikategorioita (Käyttäjät, tapahtumat, nukkumapaikat…)</t>
+  </si>
+  <si>
+    <t>Layers-valikko</t>
   </si>
 </sst>
 </file>
@@ -460,15 +478,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2CA091C-D76E-416C-82F8-D2C6C8AC4F23}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="35.42578125" customWidth="1"/>
     <col min="2" max="2" width="26.7109375" customWidth="1"/>
     <col min="3" max="3" width="29.7109375" customWidth="1"/>
     <col min="4" max="4" width="18.140625" customWidth="1"/>
@@ -537,6 +555,39 @@
         <v>13</v>
       </c>
     </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>